<commit_message>
Update Phase 1 (A1-A6) evidence.
</commit_message>
<xml_diff>
--- a/nodeiistt/evidence.xlsx
+++ b/nodeiistt/evidence.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="51">
   <si>
     <t>TeamName</t>
   </si>
@@ -92,34 +92,91 @@
     <t>ClassID</t>
   </si>
   <si>
-    <t>tx hash on irisnet</t>
-  </si>
-  <si>
-    <t>class id you issued</t>
+    <t>136AEF507B7B7256BD9400927E0BF4D7A2A97FA1BB9C0F0470EB49764BD3B438</t>
+  </si>
+  <si>
+    <t>nodeistnft</t>
   </si>
   <si>
     <t>NFTID</t>
   </si>
   <si>
-    <t>nft id you minted</t>
+    <t>6005E1551121039F197FE56E95D9AC675C54603F4DAF36067A61D72AFAFD9D18</t>
+  </si>
+  <si>
+    <t>ndstnft1</t>
+  </si>
+  <si>
+    <t>95B10B7D907C35FA5F3585BED847C0498443A94C0A3F5539D981991B1BF2E95B</t>
+  </si>
+  <si>
+    <t>ndstnft2</t>
+  </si>
+  <si>
+    <t>70AC37F5A1FCA19AEBB060875478D588C6FBEB9A45A68E374322059462D0D2E9</t>
+  </si>
+  <si>
+    <t>ndstnft3</t>
+  </si>
+  <si>
+    <t>78B4F0E8D34CADE728114A74E7E94C97BFF3A0B48F83BAE7C4AD5CAFF075AFE3</t>
+  </si>
+  <si>
+    <t>ndstnft4</t>
   </si>
   <si>
     <t>ChainID</t>
   </si>
   <si>
-    <t>ibc class on dest chain</t>
+    <t>211DFFB96FEAA8A992F550484982C63F1C8D279A4AD989467D183066F8755655</t>
+  </si>
+  <si>
+    <t>wasm.stars1ve46fjrhcrum94c7d8yc2wsdz8cpuw73503e8qn9r44spr6dw0lsvmvtqh/channel-207/nodeistnft</t>
+  </si>
+  <si>
+    <t>elgafar-1</t>
+  </si>
+  <si>
+    <t>classId:</t>
+  </si>
+  <si>
+    <t>contract(cw-721):</t>
+  </si>
+  <si>
+    <t>stars1lgfwmg4vcvjvtffhts5a35z4enk4s32lwm3r5ju05h40detmzues9w3wst</t>
+  </si>
+  <si>
+    <t>A4352C1E8F2581718A9B96F79C830444502EADD5F6AD2EFE84E8316D5E03BE7D</t>
+  </si>
+  <si>
+    <t>ibc/6180E5A0AFE554AA5CC5AEEF90BA95AB3EEE9C6B7554B45714BE30B3F6A2129B</t>
+  </si>
+  <si>
+    <t>uptick_7000-2</t>
+  </si>
+  <si>
+    <t>2F740CA1EF2C7AA80318BF7DBC5CA124240C55EECDAA800257B1A8A460C5E193</t>
+  </si>
+  <si>
+    <t>nft-transfer/channel-3/nodeistnft</t>
+  </si>
+  <si>
+    <t>collection:</t>
+  </si>
+  <si>
+    <t>7F02D26D3C822D8D13510FF4B82B73913245A634EB818E48232FBC6AC4F663DC</t>
+  </si>
+  <si>
+    <t>gon-irishub-1</t>
+  </si>
+  <si>
+    <t>555D3CFE8016FEEE10B7624EC110955FDB6956F8AC40A7982E380AFB6D0861EE</t>
+  </si>
+  <si>
+    <t>ibc class on chain</t>
   </si>
   <si>
     <t>nft id</t>
-  </si>
-  <si>
-    <t>dest chain id</t>
-  </si>
-  <si>
-    <t>tx hash on dest chain</t>
-  </si>
-  <si>
-    <t>ibc class on chain</t>
   </si>
   <si>
     <t>tx hash on that chain</t>
@@ -142,12 +199,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="27">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -165,6 +222,128 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -175,106 +354,25 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -286,7 +384,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -299,29 +397,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -344,55 +419,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -404,127 +599,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -542,16 +617,22 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -567,6 +648,15 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -587,16 +677,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -604,8 +694,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -620,164 +710,161 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1172,7 +1259,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6380952380952" defaultRowHeight="12.75" outlineLevelRow="1" outlineLevelCol="7"/>
@@ -1213,28 +1300,28 @@
       </c>
     </row>
     <row r="2" ht="14.25" spans="1:8">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="10" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1269,10 +1356,10 @@
     </row>
     <row r="2" ht="14.25" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1306,10 +1393,10 @@
     </row>
     <row r="2" ht="14.25" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1343,10 +1430,10 @@
     </row>
     <row r="2" ht="14.25" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1380,10 +1467,10 @@
     </row>
     <row r="2" ht="14.25" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1404,7 +1491,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6380952380952" defaultRowHeight="12.75" outlineLevelRow="3" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="1" max="1" width="31.4285714285714" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" spans="1:2">
@@ -1412,25 +1499,25 @@
         <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" ht="14.25" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" ht="14.25" spans="1:1">
       <c r="A3" s="3" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" ht="14.25" spans="1:1">
       <c r="A4" s="3" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1459,25 +1546,25 @@
         <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" ht="14.25" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" ht="14.25" spans="1:1">
       <c r="A3" s="3" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" ht="14.25" spans="1:1">
       <c r="A4" s="3" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1506,25 +1593,25 @@
         <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" ht="14.25" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" ht="14.25" spans="1:1">
       <c r="A3" s="3" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" ht="14.25" spans="1:1">
       <c r="A4" s="3" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1553,25 +1640,25 @@
         <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" ht="14.25" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" ht="14.25" spans="1:1">
       <c r="A3" s="3" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" ht="14.25" spans="1:1">
       <c r="A4" s="3" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1600,25 +1687,25 @@
         <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" ht="14.25" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" ht="14.25" spans="1:1">
       <c r="A3" s="3" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" ht="14.25" spans="1:1">
       <c r="A4" s="3" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1647,25 +1734,25 @@
         <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" ht="14.25" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" ht="14.25" spans="1:1">
       <c r="A3" s="3" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" ht="14.25" spans="1:1">
       <c r="A4" s="3" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1681,7 +1768,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6380952380952" defaultRowHeight="12.75" outlineLevelRow="1" outlineLevelCol="1"/>
@@ -1731,25 +1818,25 @@
         <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" ht="14.25" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" ht="14.25" spans="1:1">
       <c r="A3" s="3" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" ht="14.25" spans="1:1">
       <c r="A4" s="3" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1778,25 +1865,25 @@
         <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" ht="14.25" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" ht="14.25" spans="1:1">
       <c r="A3" s="3" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" ht="14.25" spans="1:1">
       <c r="A4" s="3" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1824,12 +1911,12 @@
     </row>
     <row r="2" ht="16.4" customHeight="1" spans="1:1">
       <c r="A2" s="2" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" ht="14.25" spans="1:1">
       <c r="A3" s="3" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1860,12 +1947,12 @@
     </row>
     <row r="2" ht="14.25" spans="1:1">
       <c r="A2" s="2" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" ht="14.25" spans="1:1">
       <c r="A3" s="3" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1896,12 +1983,12 @@
     </row>
     <row r="2" ht="14.25" spans="1:1">
       <c r="A2" s="2" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" ht="14.25" spans="1:1">
       <c r="A3" s="3" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1932,12 +2019,12 @@
     </row>
     <row r="2" ht="14.25" spans="1:1">
       <c r="A2" s="2" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" ht="14.25" spans="1:1">
       <c r="A3" s="3" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1953,13 +2040,13 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6380952380952" defaultRowHeight="12.75" outlineLevelRow="1" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="12.6380952380952" defaultRowHeight="12.75" outlineLevelRow="4" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="2" width="17.8857142857143" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
@@ -1978,13 +2065,46 @@
     </row>
     <row r="2" ht="14.25" spans="1:3">
       <c r="A2" s="3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" ht="14.25" spans="1:3">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" ht="14.25" spans="1:3">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" ht="14.25" spans="1:3">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1997,13 +2117,170 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="E4" sqref="E4:G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6380952380952" defaultRowHeight="12.75" outlineLevelRow="1" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="12.6380952380952" defaultRowHeight="12.75" outlineLevelRow="4" outlineLevelCol="5"/>
+  <cols>
+    <col min="1" max="2" width="17.8857142857143" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
+    <col min="5" max="5" width="19" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="14.25" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" ht="14.25" spans="1:4">
+      <c r="A2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" ht="15" spans="5:6">
+      <c r="E4" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" ht="14.25" spans="5:6">
+      <c r="E5" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.6380952380952" defaultRowHeight="12.75" outlineLevelCol="5"/>
+  <cols>
+    <col min="1" max="2" width="17.8857142857143" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="5" max="5" width="47.5714285714286" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="14.25" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" ht="16" customHeight="1" spans="1:4">
+      <c r="A2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" ht="14.25" spans="1:4">
+      <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" ht="12" customHeight="1" spans="5:5">
+      <c r="E4" s="9"/>
+    </row>
+    <row r="5" ht="15" spans="5:6">
+      <c r="E5" s="5"/>
+      <c r="F5" s="6"/>
+    </row>
+    <row r="6" ht="14.25" spans="5:6">
+      <c r="E6" s="7"/>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="8" ht="15" spans="5:6">
+      <c r="E8" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" ht="14.25" spans="5:6">
+      <c r="E9" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.6380952380952" defaultRowHeight="12.75" outlineLevelRow="6" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="2" width="17.8857142857143" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
@@ -2020,21 +2297,37 @@
         <v>19</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" ht="14.25" spans="1:4">
       <c r="A2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>22</v>
+        <v>41</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>30</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" ht="15" spans="5:6">
+      <c r="E6" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" ht="14.25" spans="5:6">
+      <c r="E7" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -2044,116 +2337,16 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6380952380952" defaultRowHeight="12.75" outlineLevelRow="1" outlineLevelCol="3"/>
-  <cols>
-    <col min="1" max="2" width="17.8857142857143" customWidth="1"/>
-    <col min="3" max="3" width="16" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="14.25" spans="1:4">
-      <c r="A1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" ht="14.25" spans="1:4">
-      <c r="A2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6380952380952" defaultRowHeight="12.75" outlineLevelRow="1" outlineLevelCol="3"/>
-  <cols>
-    <col min="1" max="2" width="17.8857142857143" customWidth="1"/>
-    <col min="3" max="3" width="16" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="14.25" spans="1:4">
-      <c r="A1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" ht="14.25" spans="1:4">
-      <c r="A2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6380952380952" defaultRowHeight="12.75" outlineLevelRow="1" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="12.6380952380952" defaultRowHeight="12.75" outlineLevelRow="6" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="1" width="17.8857142857143" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
@@ -2172,21 +2365,37 @@
         <v>19</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" ht="14.25" spans="1:4">
       <c r="A2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>26</v>
+        <v>43</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>36</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" ht="15" spans="5:6">
+      <c r="E6" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" ht="14.25" spans="5:6">
+      <c r="E7" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -2220,10 +2429,10 @@
     </row>
     <row r="2" ht="14.25" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -2257,10 +2466,10 @@
     </row>
     <row r="2" ht="14.25" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Phase 2 Evidence (A7-A20)
</commit_message>
<xml_diff>
--- a/nodeiistt/evidence.xlsx
+++ b/nodeiistt/evidence.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12375" tabRatio="500" activeTab="5"/>
+    <workbookView windowWidth="28800" windowHeight="12375" tabRatio="500" firstSheet="7" activeTab="20"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="90">
   <si>
     <t>TeamName</t>
   </si>
@@ -155,19 +155,154 @@
     <t>555D3CFE8016FEEE10B7624EC110955FDB6956F8AC40A7982E380AFB6D0861EE</t>
   </si>
   <si>
-    <t>ibc class on chain</t>
-  </si>
-  <si>
-    <t>nft id</t>
-  </si>
-  <si>
-    <t>tx hash on that chain</t>
-  </si>
-  <si>
-    <t>chain id</t>
-  </si>
-  <si>
-    <t>tx hash on that chain	chain id</t>
+    <t>ibc/A40CD3D0A45460B9213B21140CE6640C4AFE496F10447784FB2AC34A26D5A8E0</t>
+  </si>
+  <si>
+    <t>ibc/5EA1741B323CFE4A8C5F403E3697A8C585DCBD665605277FDA800EB746378D6C</t>
+  </si>
+  <si>
+    <t>bft5</t>
+  </si>
+  <si>
+    <t>ibc/0E5766B7D0AE8E97E314C19FA195DBDBF84EDDF2B38221EB5E8740E96C563E70</t>
+  </si>
+  <si>
+    <t>nft7</t>
+  </si>
+  <si>
+    <t>ibc/CCEFBD39B3D6E27CF0B4B61BC04B80ED293F5A31A45E6401C3206FD67951A022</t>
+  </si>
+  <si>
+    <t>nft11</t>
+  </si>
+  <si>
+    <t>ibc/12E32D8A5C370E7321BC00DB03C63799C5E610F7BC07D5005165B58F55E17ABD</t>
+  </si>
+  <si>
+    <t>nft12</t>
+  </si>
+  <si>
+    <t>ibc/673EC40CA20846995DEA232C80EC911A36D75E0537DDEDA8570D0B473BB84CD3</t>
+  </si>
+  <si>
+    <t>nft14</t>
+  </si>
+  <si>
+    <t>74D3EC284B826094734E15749482EB205EAD435FF7BAC97BECC8619375F751B6</t>
+  </si>
+  <si>
+    <t>gon-irishub-1</t>
+  </si>
+  <si>
+    <t>DA3CD7B691ED46658D85E40B9C29421B9170855839BFAD05A98E28AFAD1D0D23</t>
+  </si>
+  <si>
+    <t>A518421A8E04A2A53E50880FD4B4DF3CF08B8BE1E4E8D0CF995F55EBD3EE9304</t>
+  </si>
+  <si>
+    <t>0B15664C302875164CB52526C3978742B173EF95A33ACB859521D797BE849821</t>
+  </si>
+  <si>
+    <t>7FB882C4B8DBC11DAB0125B42470C7CBC66EBE5CA5D0A3A27357E084AEB9464C</t>
+  </si>
+  <si>
+    <t>3E2EB90244EE3A05628417144EFE9EBE9C2E8387611E386D8D17A27409681631</t>
+  </si>
+  <si>
+    <t>2185595B2F117FD011DFCFE6D267CCFD39374D9E2FDA469B530487538134B127</t>
+  </si>
+  <si>
+    <t>gon-flixnet-1</t>
+  </si>
+  <si>
+    <t>4E0336D271A8937331A1843DD251A53E1DFCEE46B72E856B30AAC34B942323DC</t>
+  </si>
+  <si>
+    <t>2CF4F048F3F47B31F4C8EC79590463CF9D12255D5FEEAD362AC1F9AEBE408A97</t>
+  </si>
+  <si>
+    <t>7F41A20BBEC64B1A65D68A7C44E831D98B8B1C5CB9FA3472AA8152D224846A7A</t>
+  </si>
+  <si>
+    <t>uni-6</t>
+  </si>
+  <si>
+    <t>B4E94384FCABCB66FC732E886105F4BB6BE73E21C22B36CF0C0EAD5A9FF9241F</t>
+  </si>
+  <si>
+    <t>166775EB00EAAA17908771BCCD6291EDDB6FF17EF56735A08EE4C51EE01C4377</t>
+  </si>
+  <si>
+    <t>F31B00F6D859ECDD50EE438C4D540D86973D9E04D66BDEB5867C2374AA4E41A6</t>
+  </si>
+  <si>
+    <t>38EBFD447A44D685921A06A933A845D337EC9483C996D869E9AE3D46EC428199</t>
+  </si>
+  <si>
+    <t>5F92D251FF8B103E0137866F767E483D34B4C9F6A5B90D666A79D2343724793A</t>
+  </si>
+  <si>
+    <t>60FC80740C5E50D3EAF966AF08166695DF18E9CA922E68192782CE19215F9C7B</t>
+  </si>
+  <si>
+    <t>5E2A6BC5FC790C305D473F62289805CE28A5DDBC42458119452807F159C50009</t>
+  </si>
+  <si>
+    <t>E0F99AB2B759BAE79F948CEFF6DE333083172C03F8BEB3039974DB106223B475</t>
+  </si>
+  <si>
+    <t>0FE2DF28561D08C200499A86CEC4358D297CCEF794114233291525E8F3CDC5E8</t>
+  </si>
+  <si>
+    <t>90150589F5AE9A7C3A8BBD4086BEC7F8CAF8F7045EE64BDAA8AAB616BE452B85</t>
+  </si>
+  <si>
+    <t>CE2310D14C4D7B12A5E55A8BFEBCC8B9B58B431CAD9CBE03727A5EEA4B2C0DD3</t>
+  </si>
+  <si>
+    <t>9E090DD29941F50214F5407F244B0D4C7FBBADBCCFBBF4A399353E9BE2005FAE</t>
+  </si>
+  <si>
+    <t>7F1E7E28FC1BEC1E91310B1105BB3227A907987C976D826F95EA31C227355934</t>
+  </si>
+  <si>
+    <t>721365573AD8DFC787B59E129EAC719721D0756C1B4D906BE8C9D3BF0DE93D3C</t>
+  </si>
+  <si>
+    <t>C8A81CE45FD5034E89755F3516F38D864945B06C1D9DD311721AC866230212E5</t>
+  </si>
+  <si>
+    <t>1819C5B936B96F49DD5CDE493F9F7884E033D699D309664071BA185873C8643B</t>
+  </si>
+  <si>
+    <t>A25D286C8CD22151C0BC035BC540BF3E9534CD518FEFD84437EBCD21995FFCD5</t>
+  </si>
+  <si>
+    <t>C8506B5B62019679382ECC108DF4646CF13BFDC4B1917325FD12668518590722</t>
+  </si>
+  <si>
+    <t>8BC5AEE0ECCCADE21C8C3D23878710F50CDF83AB823E80E0E375597941AD6334</t>
+  </si>
+  <si>
+    <t>F2C58D765C48BFE8B76623A2D078A1E1064FE95311FAB62D9C59244C938485C3</t>
+  </si>
+  <si>
+    <t>8C96BBA8DA57CB120F3EA05F92F553CFD250AE4DE3803CA0129740D02D6A93C3</t>
+  </si>
+  <si>
+    <t>4DBF8282A025CDADEE288F9A047293B32C9DE5F849F348207F55AB2AD0CB95EF</t>
+  </si>
+  <si>
+    <t>B29194C8EB524A948F0898CEE5270709411A298FD9B1ABAA6B36612866BF7075</t>
+  </si>
+  <si>
+    <t>D71FA15A830E6C0C3FDF147672A1BDF2EACBD0BF9CF8D0F5FDBD9ADA75ABD731</t>
+  </si>
+  <si>
+    <t>07B9C23D5233F0850FE6D466A180929DD4C012A980DE6BDD3FE9849F797D923F</t>
+  </si>
+  <si>
+    <t>CAF9BD1AEE10E07A26C2178287AEFD443C70B4FFD40EABFF17DCD8BAC12A72A5</t>
   </si>
   <si>
     <t>The first Interchain NFT-Transfer TxHash</t>
@@ -213,7 +348,26 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -221,7 +375,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -235,36 +389,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -287,16 +413,16 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -308,8 +434,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -332,14 +459,23 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -353,9 +489,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -389,13 +524,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -407,169 +674,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -580,30 +715,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -632,21 +743,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -670,6 +766,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -680,149 +791,177 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -832,9 +971,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1229,7 +1365,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6380952380952" defaultRowHeight="12.75" outlineLevelRow="1" outlineLevelCol="7"/>
@@ -1270,28 +1406,28 @@
       </c>
     </row>
     <row r="2" ht="14.25" spans="1:8">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="H2" s="11" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1308,7 +1444,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6380952380952" defaultRowHeight="12.75" outlineLevelRow="1" outlineLevelCol="1"/>
@@ -1326,10 +1462,10 @@
     </row>
     <row r="2" ht="14.25" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1345,7 +1481,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6380952380952" defaultRowHeight="12.75" outlineLevelRow="1" outlineLevelCol="1"/>
@@ -1363,10 +1499,10 @@
     </row>
     <row r="2" ht="14.25" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1382,7 +1518,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6380952380952" defaultRowHeight="12.75" outlineLevelRow="1" outlineLevelCol="1"/>
@@ -1400,10 +1536,10 @@
     </row>
     <row r="2" ht="14.25" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1419,7 +1555,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6380952380952" defaultRowHeight="12.75" outlineLevelRow="1" outlineLevelCol="1"/>
@@ -1437,10 +1573,10 @@
     </row>
     <row r="2" ht="14.25" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1453,13 +1589,13 @@
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6380952380952" defaultRowHeight="12.75" outlineLevelRow="3" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="12.6380952380952" defaultRowHeight="12.75" outlineLevelRow="4" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="31.4285714285714" customWidth="1"/>
   </cols>
@@ -1474,20 +1610,34 @@
     </row>
     <row r="2" ht="14.25" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" ht="14.25" spans="1:1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" ht="14.25" spans="1:2">
       <c r="A3" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" ht="14.25" spans="1:1">
+        <v>51</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" ht="14.25" spans="1:2">
       <c r="A4" s="3" t="s">
-        <v>42</v>
+        <v>52</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" ht="14.25" spans="1:2">
+      <c r="A5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1500,13 +1650,13 @@
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6380952380952" defaultRowHeight="12.75" outlineLevelRow="3" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="12.6380952380952" defaultRowHeight="12.75" outlineLevelRow="4" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
   </cols>
@@ -1521,20 +1671,34 @@
     </row>
     <row r="2" ht="14.25" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" ht="14.25" spans="1:1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" ht="14.25" spans="1:2">
       <c r="A3" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" ht="14.25" spans="1:1">
+        <v>55</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" ht="14.25" spans="1:2">
       <c r="A4" s="3" t="s">
-        <v>42</v>
+        <v>56</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1547,13 +1711,13 @@
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6380952380952" defaultRowHeight="12.75" outlineLevelRow="3" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="12.6380952380952" defaultRowHeight="12.75" outlineLevelRow="4" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
   </cols>
@@ -1568,20 +1732,34 @@
     </row>
     <row r="2" ht="14.25" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" ht="14.25" spans="1:1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" ht="14.25" spans="1:2">
       <c r="A3" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" ht="14.25" spans="1:1">
+        <v>60</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" ht="14.25" spans="1:2">
       <c r="A4" s="3" t="s">
-        <v>42</v>
+        <v>62</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" ht="14.25" spans="1:2">
+      <c r="A5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1594,13 +1772,13 @@
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6380952380952" defaultRowHeight="12.75" outlineLevelRow="3" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="12.6380952380952" defaultRowHeight="12.75" outlineLevelRow="4" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
   </cols>
@@ -1615,20 +1793,34 @@
     </row>
     <row r="2" ht="14.25" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" ht="14.25" spans="1:1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" ht="14.25" spans="1:2">
       <c r="A3" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" ht="14.25" spans="1:1">
+        <v>65</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" ht="14.25" spans="1:2">
       <c r="A4" s="3" t="s">
-        <v>42</v>
+        <v>66</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" ht="14.25" spans="1:2">
+      <c r="A5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1641,13 +1833,13 @@
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6380952380952" defaultRowHeight="12.75" outlineLevelRow="3" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="12.6380952380952" defaultRowHeight="12.75" outlineLevelRow="4" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
   </cols>
@@ -1662,20 +1854,34 @@
     </row>
     <row r="2" ht="14.25" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>40</v>
+        <v>68</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" ht="14.25" spans="1:1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" ht="14.25" spans="1:2">
       <c r="A3" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" ht="14.25" spans="1:1">
+        <v>69</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" ht="14.25" spans="1:2">
       <c r="A4" s="3" t="s">
-        <v>42</v>
+        <v>70</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" ht="14.25" spans="1:2">
+      <c r="A5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1688,13 +1894,13 @@
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6380952380952" defaultRowHeight="12.75" outlineLevelRow="3" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="12.6380952380952" defaultRowHeight="12.75" outlineLevelRow="4" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
   </cols>
@@ -1709,20 +1915,34 @@
     </row>
     <row r="2" ht="14.25" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>40</v>
+        <v>72</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" ht="14.25" spans="1:1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" ht="14.25" spans="1:2">
       <c r="A3" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" ht="14.25" spans="1:1">
+        <v>73</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" ht="14.25" spans="1:2">
       <c r="A4" s="3" t="s">
-        <v>42</v>
+        <v>74</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" ht="14.25" spans="1:2">
+      <c r="A5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1772,13 +1992,13 @@
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6380952380952" defaultRowHeight="12.75" outlineLevelRow="3" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="12.6380952380952" defaultRowHeight="12.75" outlineLevelRow="6" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
   </cols>
@@ -1793,20 +2013,50 @@
     </row>
     <row r="2" ht="14.25" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>40</v>
+        <v>76</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" ht="14.25" spans="1:1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" ht="14.25" spans="1:2">
       <c r="A3" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" ht="14.25" spans="1:1">
+        <v>77</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" ht="14.25" spans="1:2">
       <c r="A4" s="3" t="s">
-        <v>42</v>
+        <v>78</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" ht="14.25" spans="1:2">
+      <c r="A6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" ht="14.25" spans="1:2">
+      <c r="A7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1819,13 +2069,13 @@
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6380952380952" defaultRowHeight="12.75" outlineLevelRow="3" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="12.6380952380952" defaultRowHeight="12.75" outlineLevelRow="6" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
   </cols>
@@ -1840,20 +2090,50 @@
     </row>
     <row r="2" ht="14.25" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>40</v>
+        <v>82</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" ht="14.25" spans="1:1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" ht="14.25" spans="1:2">
       <c r="A3" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" ht="14.25" spans="1:1">
+        <v>83</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" ht="14.25" spans="1:2">
       <c r="A4" s="3" t="s">
-        <v>42</v>
+        <v>84</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" ht="14.25" spans="1:2">
+      <c r="A5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" ht="14.25" spans="1:2">
+      <c r="A6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1881,12 +2161,12 @@
     </row>
     <row r="2" ht="16.4" customHeight="1" spans="1:1">
       <c r="A2" s="2" t="s">
-        <v>43</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" ht="14.25" spans="1:1">
       <c r="A3" s="3" t="s">
-        <v>44</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -1917,12 +2197,12 @@
     </row>
     <row r="2" ht="14.25" spans="1:1">
       <c r="A2" s="2" t="s">
-        <v>43</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" ht="14.25" spans="1:1">
       <c r="A3" s="3" t="s">
-        <v>44</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -1953,12 +2233,12 @@
     </row>
     <row r="2" ht="14.25" spans="1:1">
       <c r="A2" s="2" t="s">
-        <v>43</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" ht="14.25" spans="1:1">
       <c r="A3" s="3" t="s">
-        <v>44</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -1989,12 +2269,12 @@
     </row>
     <row r="2" ht="14.25" spans="1:1">
       <c r="A2" s="2" t="s">
-        <v>43</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" ht="14.25" spans="1:1">
       <c r="A3" s="3" t="s">
-        <v>44</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -2124,17 +2404,17 @@
       <c r="C2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="7" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="4" ht="15" spans="5:6">
-      <c r="E4" s="6"/>
-      <c r="F4" s="7"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="9"/>
     </row>
     <row r="5" ht="14.25" spans="5:6">
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
@@ -2184,7 +2464,7 @@
       <c r="C2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="7" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2198,28 +2478,28 @@
       <c r="C3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="7" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="4" ht="12" customHeight="1" spans="5:5">
-      <c r="E4" s="9"/>
+      <c r="E4" s="4"/>
     </row>
     <row r="5" ht="15" spans="5:6">
-      <c r="E5" s="6"/>
-      <c r="F5" s="7"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="9"/>
     </row>
     <row r="6" ht="14.25" spans="5:6">
-      <c r="E6" s="8"/>
-      <c r="F6" s="4"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="6"/>
     </row>
     <row r="8" ht="15" spans="5:6">
-      <c r="E8" s="6"/>
-      <c r="F8" s="7"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="9"/>
     </row>
     <row r="9" ht="14.25" spans="5:6">
-      <c r="E9" s="8"/>
-      <c r="F9" s="4"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
@@ -2233,7 +2513,7 @@
   <sheetPr/>
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
@@ -2261,23 +2541,23 @@
       <c r="A2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="6" t="s">
         <v>30</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="7" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="6" ht="15" spans="5:6">
-      <c r="E6" s="6"/>
-      <c r="F6" s="7"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="9"/>
     </row>
     <row r="7" ht="14.25" spans="5:6">
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
@@ -2321,23 +2601,23 @@
       <c r="A2" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="6" t="s">
         <v>33</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="7" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="6" ht="15" spans="5:6">
-      <c r="E6" s="6"/>
-      <c r="F6" s="7"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="9"/>
     </row>
     <row r="7" ht="14.25" spans="5:6">
-      <c r="E7" s="8"/>
-      <c r="F7" s="4"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
@@ -2352,7 +2632,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6380952380952" defaultRowHeight="12.75" outlineLevelRow="1" outlineLevelCol="1"/>
@@ -2373,7 +2653,7 @@
         <v>38</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -2389,7 +2669,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6380952380952" defaultRowHeight="12.75" outlineLevelRow="1" outlineLevelCol="1"/>
@@ -2407,10 +2687,10 @@
     </row>
     <row r="2" ht="14.25" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed revisit evidence b1-4
</commit_message>
<xml_diff>
--- a/nodeiistt/evidence.xlsx
+++ b/nodeiistt/evidence.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12375" tabRatio="500" firstSheet="7" activeTab="20"/>
+    <workbookView windowWidth="28800" windowHeight="12375" tabRatio="500" firstSheet="3" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -188,61 +188,61 @@
     <t>nft14</t>
   </si>
   <si>
-    <t>74D3EC284B826094734E15749482EB205EAD435FF7BAC97BECC8619375F751B6</t>
+    <t>68046EECE48FF1D6F4AEA64F48A02122F25E7511061DA394940AB70FDB38C1A4</t>
   </si>
   <si>
     <t>gon-irishub-1</t>
   </si>
   <si>
-    <t>DA3CD7B691ED46658D85E40B9C29421B9170855839BFAD05A98E28AFAD1D0D23</t>
-  </si>
-  <si>
-    <t>A518421A8E04A2A53E50880FD4B4DF3CF08B8BE1E4E8D0CF995F55EBD3EE9304</t>
-  </si>
-  <si>
-    <t>0B15664C302875164CB52526C3978742B173EF95A33ACB859521D797BE849821</t>
-  </si>
-  <si>
-    <t>7FB882C4B8DBC11DAB0125B42470C7CBC66EBE5CA5D0A3A27357E084AEB9464C</t>
-  </si>
-  <si>
-    <t>3E2EB90244EE3A05628417144EFE9EBE9C2E8387611E386D8D17A27409681631</t>
-  </si>
-  <si>
-    <t>2185595B2F117FD011DFCFE6D267CCFD39374D9E2FDA469B530487538134B127</t>
+    <t>087B9902304C62F6A80F1F9EBFEAE7B09EB9052FCC91ADA1F9F8062F3DCAD551</t>
+  </si>
+  <si>
+    <t>2D1050189F14D1781653007AC3EBAD59F8615380C0415380F3E16C681BA9FA95</t>
+  </si>
+  <si>
+    <t>2D4089B5C8B6D4C7A9093385AE9913D25ECABE4E426665A683E2EA09E3E67463</t>
+  </si>
+  <si>
+    <t>B75078B3B5405A1BF4B0640F2678B8E4790EC1577E7E39AF296EFEA832278665</t>
+  </si>
+  <si>
+    <t>09E23A0E24DC5D175E8A087D564B4F70D2CDEBEA988E0097412B3014157E7491</t>
+  </si>
+  <si>
+    <t>317AE14B4807351AB5771315703C98D8EB1F8CACF7F2F9057B3C02FD3576122C</t>
   </si>
   <si>
     <t>gon-flixnet-1</t>
   </si>
   <si>
-    <t>4E0336D271A8937331A1843DD251A53E1DFCEE46B72E856B30AAC34B942323DC</t>
-  </si>
-  <si>
-    <t>2CF4F048F3F47B31F4C8EC79590463CF9D12255D5FEEAD362AC1F9AEBE408A97</t>
-  </si>
-  <si>
-    <t>7F41A20BBEC64B1A65D68A7C44E831D98B8B1C5CB9FA3472AA8152D224846A7A</t>
+    <t>856E287ADEBB374DBC63F5AFDC022622AE8CD3AE1B77EAC04EED2556A88F99AC</t>
+  </si>
+  <si>
+    <t>7EA30B964E5CE0574487657D3CBDEFBE3E5B42810F3B2040B2F9904ADC43CA34</t>
+  </si>
+  <si>
+    <t>E9988C4077F43A4F7CC53D396F58C16B58083BDDA87E2C874F43F66792E7483C</t>
   </si>
   <si>
     <t>uni-6</t>
   </si>
   <si>
-    <t>B4E94384FCABCB66FC732E886105F4BB6BE73E21C22B36CF0C0EAD5A9FF9241F</t>
-  </si>
-  <si>
-    <t>166775EB00EAAA17908771BCCD6291EDDB6FF17EF56735A08EE4C51EE01C4377</t>
-  </si>
-  <si>
-    <t>F31B00F6D859ECDD50EE438C4D540D86973D9E04D66BDEB5867C2374AA4E41A6</t>
-  </si>
-  <si>
-    <t>38EBFD447A44D685921A06A933A845D337EC9483C996D869E9AE3D46EC428199</t>
-  </si>
-  <si>
-    <t>5F92D251FF8B103E0137866F767E483D34B4C9F6A5B90D666A79D2343724793A</t>
-  </si>
-  <si>
-    <t>60FC80740C5E50D3EAF966AF08166695DF18E9CA922E68192782CE19215F9C7B</t>
+    <t>6F003389C760F2D643858DAD44D50FCED3E82C593B5F2C7B2257E1E2B1B60602</t>
+  </si>
+  <si>
+    <t>13BD44F1E9E9F56594D1083E89DD2C8A5254A4FE28D1DF0C9F7D6F5BD7DEB2E9</t>
+  </si>
+  <si>
+    <t>101208112FBEC58317FFA4C7B6B158E17D7A536DCBCB4A0982ED22D5D3CDF272</t>
+  </si>
+  <si>
+    <t>97CB3B41F946FA191DE41F4AE8CDEDBC3399BE6164B2EA8F5112441946406506</t>
+  </si>
+  <si>
+    <t>CC23BCC18BDCF78FD4DDE6E28F9CA2BED734078E641C32992116A5FE1C0A9B89</t>
+  </si>
+  <si>
+    <t>F833C629C3DF41D1B4514E9874B5C2C9409B92163E2A2A24EF9EFEB72FA10EDB</t>
   </si>
   <si>
     <t>5E2A6BC5FC790C305D473F62289805CE28A5DDBC42458119452807F159C50009</t>
@@ -318,8 +318,8 @@
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -348,6 +348,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -359,23 +366,17 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -389,16 +390,25 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -434,22 +444,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -473,9 +467,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -490,14 +490,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -524,13 +524,127 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -542,7 +656,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -554,13 +680,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -572,139 +698,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -715,6 +715,30 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -729,15 +753,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -792,21 +807,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -818,138 +818,138 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1365,7 +1365,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6380952380952" defaultRowHeight="12.75" outlineLevelRow="1" outlineLevelCol="7"/>
@@ -1592,7 +1592,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6380952380952" defaultRowHeight="12.75" outlineLevelRow="4" outlineLevelCol="1"/>
@@ -1653,7 +1653,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6380952380952" defaultRowHeight="12.75" outlineLevelRow="4" outlineLevelCol="1"/>
@@ -1714,7 +1714,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6380952380952" defaultRowHeight="12.75" outlineLevelRow="4" outlineLevelCol="1"/>
@@ -1774,8 +1774,8 @@
   <sheetPr/>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6380952380952" defaultRowHeight="12.75" outlineLevelRow="4" outlineLevelCol="1"/>
@@ -2071,7 +2071,7 @@
   <sheetPr/>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
B1 Fail - B2 Done
</commit_message>
<xml_diff>
--- a/nodeiistt/evidence.xlsx
+++ b/nodeiistt/evidence.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12375" activeTab="2"/>
+    <workbookView windowWidth="24225" windowHeight="12375" firstSheet="9" activeTab="22"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="90">
   <si>
     <t>TeamName</t>
   </si>
@@ -302,6 +302,12 @@
   </si>
   <si>
     <t>The Internal Transfer TxHash on IRISnet</t>
+  </si>
+  <si>
+    <t>850AC11E7C7AE890AADD68E76FF5EC76A971C7035BC83C8E741DBD5861136443</t>
+  </si>
+  <si>
+    <t>C494F419998694B960F2254AF4A06587E96D34BC10B8FAF2522A5FAB76D44BED</t>
   </si>
 </sst>
 </file>
@@ -309,10 +315,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -341,22 +347,31 @@
       <charset val="1"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -372,39 +387,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -418,28 +401,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -448,8 +409,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -462,8 +424,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -484,6 +447,49 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -506,43 +512,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -554,139 +686,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -716,27 +722,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -756,35 +751,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -806,16 +777,51 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -833,130 +839,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1338,7 +1344,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="7"/>
@@ -2178,7 +2184,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="2"/>
@@ -2214,8 +2220,8 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="2"/>
@@ -2230,12 +2236,12 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:1">
       <c r="A2" s="3" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:1">
       <c r="A3" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -2325,8 +2331,8 @@
   </sheetPr>
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K39" sqref="K39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="2"/>

</xml_diff>